<commit_message>
Working on parallel processing...
</commit_message>
<xml_diff>
--- a/sample_output/asquant_group1_Vs_group2.xlsx
+++ b/sample_output/asquant_group1_Vs_group2.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="12">
   <si>
     <t>chrom</t>
   </si>
@@ -54,39 +54,6 @@
   </si>
   <si>
     <t>chromRegionLLong</t>
-  </si>
-  <si>
-    <t>chr10</t>
-  </si>
-  <si>
-    <t>TPD52L1</t>
-  </si>
-  <si>
-    <t>TRMT11</t>
-  </si>
-  <si>
-    <t>ZUFSP</t>
-  </si>
-  <si>
-    <t>chr10:TPD52L1:31343011-31343026</t>
-  </si>
-  <si>
-    <t>chr10:TRMT11:30591020-30591102</t>
-  </si>
-  <si>
-    <t>chr10:TPD52L1:31341139-31341178</t>
-  </si>
-  <si>
-    <t>chr10:TPD52L1:31338184-31338245</t>
-  </si>
-  <si>
-    <t>chr10:ZUFSP:33935088-33935257</t>
-  </si>
-  <si>
-    <t>NCOA7</t>
-  </si>
-  <si>
-    <t>chr10:NCOA7:30691755-30691787</t>
   </si>
 </sst>
 </file>
@@ -444,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,196 +453,6 @@
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <v>31343011</v>
-      </c>
-      <c r="D2">
-        <v>31343026</v>
-      </c>
-      <c r="E2">
-        <v>0.0375962913753642</v>
-      </c>
-      <c r="F2">
-        <v>-0.2443458799799822</v>
-      </c>
-      <c r="G2">
-        <v>0.2443458799799822</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>22.72291993720565</v>
-      </c>
-      <c r="J2">
-        <v>9.4375</v>
-      </c>
-      <c r="K2">
-        <v>29.18602825745682</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3">
-        <v>30591020</v>
-      </c>
-      <c r="D3">
-        <v>30591102</v>
-      </c>
-      <c r="E3">
-        <v>0.6811682297322682</v>
-      </c>
-      <c r="F3">
-        <v>0.0459023371929579</v>
-      </c>
-      <c r="G3">
-        <v>0.0459023371929579</v>
-      </c>
-      <c r="H3">
-        <v>70.74698795180723</v>
-      </c>
-      <c r="I3">
-        <v>92.98034076015728</v>
-      </c>
-      <c r="J3">
-        <v>73.4578313253012</v>
-      </c>
-      <c r="K3">
-        <v>116.7487986020096</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4">
-        <v>31341139</v>
-      </c>
-      <c r="D4">
-        <v>31341178</v>
-      </c>
-      <c r="E4">
-        <v>0.759639026899154</v>
-      </c>
-      <c r="F4">
-        <v>-0.0710106975581275</v>
-      </c>
-      <c r="G4">
-        <v>0.0710106975581275</v>
-      </c>
-      <c r="H4">
-        <v>3.425</v>
-      </c>
-      <c r="I4">
-        <v>23.0496</v>
-      </c>
-      <c r="J4">
-        <v>7.425</v>
-      </c>
-      <c r="K4">
-        <v>29.6296</v>
-      </c>
-      <c r="L4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>31338184</v>
-      </c>
-      <c r="D5">
-        <v>31338245</v>
-      </c>
-      <c r="E5">
-        <v>0.8905158238694521</v>
-      </c>
-      <c r="F5">
-        <v>0.0510201852206924</v>
-      </c>
-      <c r="G5">
-        <v>0.0510201852206924</v>
-      </c>
-      <c r="H5">
-        <v>11.20967741935484</v>
-      </c>
-      <c r="I5">
-        <v>23.00814332247557</v>
-      </c>
-      <c r="J5">
-        <v>11.40322580645161</v>
-      </c>
-      <c r="K5">
-        <v>29.82654723127036</v>
-      </c>
-      <c r="L5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>33935088</v>
-      </c>
-      <c r="D6">
-        <v>33935257</v>
-      </c>
-      <c r="E6">
-        <v>0.9533697673964592</v>
-      </c>
-      <c r="F6">
-        <v>-0.0213551662639566</v>
-      </c>
-      <c r="G6">
-        <v>0.0213551662639566</v>
-      </c>
-      <c r="H6">
-        <v>41.96470588235294</v>
-      </c>
-      <c r="I6">
-        <v>54.60894308943089</v>
-      </c>
-      <c r="J6">
-        <v>50.81764705882353</v>
-      </c>
-      <c r="K6">
-        <v>60.65121951219512</v>
-      </c>
-      <c r="L6" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -787,7 +564,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -829,44 +606,6 @@
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2">
-        <v>30691755</v>
-      </c>
-      <c r="D2">
-        <v>30691787</v>
-      </c>
-      <c r="E2">
-        <v>0.8698350074869731</v>
-      </c>
-      <c r="F2">
-        <v>0.026160299348494</v>
-      </c>
-      <c r="G2">
-        <v>0.026160299348494</v>
-      </c>
-      <c r="H2">
-        <v>88.33333333333333</v>
-      </c>
-      <c r="I2">
-        <v>95.53465184700885</v>
-      </c>
-      <c r="J2">
-        <v>102.7272727272727</v>
-      </c>
-      <c r="K2">
-        <v>123.4163125204315</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Working on parallel processing..."
This reverts commit f7730657dc1aad11920e127a2a1ebe05e4cd9d97.
</commit_message>
<xml_diff>
--- a/sample_output/asquant_group1_Vs_group2.xlsx
+++ b/sample_output/asquant_group1_Vs_group2.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="23">
   <si>
     <t>chrom</t>
   </si>
@@ -54,6 +54,39 @@
   </si>
   <si>
     <t>chromRegionLLong</t>
+  </si>
+  <si>
+    <t>chr10</t>
+  </si>
+  <si>
+    <t>TPD52L1</t>
+  </si>
+  <si>
+    <t>TRMT11</t>
+  </si>
+  <si>
+    <t>ZUFSP</t>
+  </si>
+  <si>
+    <t>chr10:TPD52L1:31343011-31343026</t>
+  </si>
+  <si>
+    <t>chr10:TRMT11:30591020-30591102</t>
+  </si>
+  <si>
+    <t>chr10:TPD52L1:31341139-31341178</t>
+  </si>
+  <si>
+    <t>chr10:TPD52L1:31338184-31338245</t>
+  </si>
+  <si>
+    <t>chr10:ZUFSP:33935088-33935257</t>
+  </si>
+  <si>
+    <t>NCOA7</t>
+  </si>
+  <si>
+    <t>chr10:NCOA7:30691755-30691787</t>
   </si>
 </sst>
 </file>
@@ -411,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -453,6 +486,196 @@
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>31343011</v>
+      </c>
+      <c r="D2">
+        <v>31343026</v>
+      </c>
+      <c r="E2">
+        <v>0.0375962913753642</v>
+      </c>
+      <c r="F2">
+        <v>-0.2443458799799822</v>
+      </c>
+      <c r="G2">
+        <v>0.2443458799799822</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>22.72291993720565</v>
+      </c>
+      <c r="J2">
+        <v>9.4375</v>
+      </c>
+      <c r="K2">
+        <v>29.18602825745682</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>30591020</v>
+      </c>
+      <c r="D3">
+        <v>30591102</v>
+      </c>
+      <c r="E3">
+        <v>0.6811682297322682</v>
+      </c>
+      <c r="F3">
+        <v>0.0459023371929579</v>
+      </c>
+      <c r="G3">
+        <v>0.0459023371929579</v>
+      </c>
+      <c r="H3">
+        <v>70.74698795180723</v>
+      </c>
+      <c r="I3">
+        <v>92.98034076015728</v>
+      </c>
+      <c r="J3">
+        <v>73.4578313253012</v>
+      </c>
+      <c r="K3">
+        <v>116.7487986020096</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>31341139</v>
+      </c>
+      <c r="D4">
+        <v>31341178</v>
+      </c>
+      <c r="E4">
+        <v>0.759639026899154</v>
+      </c>
+      <c r="F4">
+        <v>-0.0710106975581275</v>
+      </c>
+      <c r="G4">
+        <v>0.0710106975581275</v>
+      </c>
+      <c r="H4">
+        <v>3.425</v>
+      </c>
+      <c r="I4">
+        <v>23.0496</v>
+      </c>
+      <c r="J4">
+        <v>7.425</v>
+      </c>
+      <c r="K4">
+        <v>29.6296</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>31338184</v>
+      </c>
+      <c r="D5">
+        <v>31338245</v>
+      </c>
+      <c r="E5">
+        <v>0.8905158238694521</v>
+      </c>
+      <c r="F5">
+        <v>0.0510201852206924</v>
+      </c>
+      <c r="G5">
+        <v>0.0510201852206924</v>
+      </c>
+      <c r="H5">
+        <v>11.20967741935484</v>
+      </c>
+      <c r="I5">
+        <v>23.00814332247557</v>
+      </c>
+      <c r="J5">
+        <v>11.40322580645161</v>
+      </c>
+      <c r="K5">
+        <v>29.82654723127036</v>
+      </c>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>33935088</v>
+      </c>
+      <c r="D6">
+        <v>33935257</v>
+      </c>
+      <c r="E6">
+        <v>0.9533697673964592</v>
+      </c>
+      <c r="F6">
+        <v>-0.0213551662639566</v>
+      </c>
+      <c r="G6">
+        <v>0.0213551662639566</v>
+      </c>
+      <c r="H6">
+        <v>41.96470588235294</v>
+      </c>
+      <c r="I6">
+        <v>54.60894308943089</v>
+      </c>
+      <c r="J6">
+        <v>50.81764705882353</v>
+      </c>
+      <c r="K6">
+        <v>60.65121951219512</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -564,7 +787,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -606,6 +829,44 @@
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>30691755</v>
+      </c>
+      <c r="D2">
+        <v>30691787</v>
+      </c>
+      <c r="E2">
+        <v>0.8698350074869731</v>
+      </c>
+      <c r="F2">
+        <v>0.026160299348494</v>
+      </c>
+      <c r="G2">
+        <v>0.026160299348494</v>
+      </c>
+      <c r="H2">
+        <v>88.33333333333333</v>
+      </c>
+      <c r="I2">
+        <v>95.53465184700885</v>
+      </c>
+      <c r="J2">
+        <v>102.7272727272727</v>
+      </c>
+      <c r="K2">
+        <v>123.4163125204315</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds cpu pooling in MakeFullDictionary
</commit_message>
<xml_diff>
--- a/sample_output/asquant_group1_Vs_group2.xlsx
+++ b/sample_output/asquant_group1_Vs_group2.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="21">
   <si>
     <t>chrom</t>
   </si>
@@ -81,12 +81,6 @@
   </si>
   <si>
     <t>chr10:ZUFSP:33935088-33935257</t>
-  </si>
-  <si>
-    <t>NCOA7</t>
-  </si>
-  <si>
-    <t>chr10:NCOA7:30691755-30691787</t>
   </si>
 </sst>
 </file>
@@ -787,7 +781,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -829,44 +823,6 @@
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2">
-        <v>30691755</v>
-      </c>
-      <c r="D2">
-        <v>30691787</v>
-      </c>
-      <c r="E2">
-        <v>0.8698350074869731</v>
-      </c>
-      <c r="F2">
-        <v>0.026160299348494</v>
-      </c>
-      <c r="G2">
-        <v>0.026160299348494</v>
-      </c>
-      <c r="H2">
-        <v>88.33333333333333</v>
-      </c>
-      <c r="I2">
-        <v>95.53465184700885</v>
-      </c>
-      <c r="J2">
-        <v>102.7272727272727</v>
-      </c>
-      <c r="K2">
-        <v>123.4163125204315</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>